<commit_message>
Update cube metadata: Package4
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010027-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010027-A-TC-TM-TP.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Informe-05-050314-A-TC-TP" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Informe-01-010027-A-TC-TM-TP" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -328,31 +328,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:U6"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="45.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="45.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="57.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="57.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="47.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="58.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="50.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="38.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,6 +682,9 @@
         <v>66</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>